<commit_message>
Added link to Harry's solution
</commit_message>
<xml_diff>
--- a/VHX-Lookup_Functions_Case.xlsx
+++ b/VHX-Lookup_Functions_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE27B4F-6978-45C3-B6D0-D00822AF8968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EDE29B-6E35-4DAC-9EBF-171F92BFB530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="231">
   <si>
     <t>Case Author</t>
   </si>
@@ -867,6 +867,9 @@
   </si>
   <si>
     <t>Not Found</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hM0G2_cE_TE</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1871,7 @@
   <dimension ref="A1:O306"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E212" sqref="E212"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -1906,7 +1909,9 @@
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>230</v>
+      </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>

</xml_diff>